<commit_message>
Alteracao em algumas planilhas realizadas em aula, relevando um cuidado maior com conteudos academicos e seus devidos direitos autorais
</commit_message>
<xml_diff>
--- a/planilhas-comuns/origens-e-aplicacoes.xlsx
+++ b/planilhas-comuns/origens-e-aplicacoes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lopes\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Portfólio\estudos-planilhas\planilhas-comuns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7987848-8FEE-41A1-8DCF-6A1E6A060651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3922701B-FCEA-44E1-B51C-0FA541053B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{5621AAAE-5E8A-43F1-AEC5-8670B457ABFA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
   <si>
     <t>TRANSAÇÃO 1</t>
   </si>
@@ -213,9 +213,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>ATIVIDADES</t>
   </si>
 </sst>
 </file>
@@ -942,20 +939,11 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -997,9 +985,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1030,15 +1015,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="25" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1090,44 +1066,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="31" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1150,15 +1090,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="15" fillId="6" borderId="40" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="15" fillId="6" borderId="41" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="40% - Ênfase5" xfId="8" builtinId="47"/>
@@ -1296,473 +1285,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>16566</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>8283</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>16565</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Retângulo 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E41B2707-A851-67E7-200D-57923DF0F830}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="612913" y="2932044"/>
-          <a:ext cx="5334000" cy="6129130"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>B -) </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Em termos percentuais, o Patrimônio Líquido contribuiu para formar quantos dos ativos da empresa? O que isso quer dizer?</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>R: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>O Patrimônio Líquido ajudou a criar “Imóveis” e “Banco do Brasil C/C”, compondo assim R$ 1600, 00 de um total de R$ 2.550,00 de ativos, sendo aproximadamente 62% do total de ativos. Isso quer dizer que a maior parte do dinheiro veio dos sócios e não de outras fontes.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>C -) </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Quais são os ativos de maior liquidez, ou seja, que tem maior facilidade de transformação em dinheiro.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>R: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>O ativo com maior liquidez sem dúvidas são as mercadorias para revenda, os estoques. Depois dele vem os imóveis e veículos que também podem ser vendidos em troca de dinheiro.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:endParaRPr lang="pt-BR" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>D -) </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Na sua visão, a empresa consegue pagar suas dívidas com facilidade ou não? Justifique a sua resposta.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>R: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Com base em minha análise, considerando que os sócios têm a maior participação na construção dos ativos, a empresa teria mais dificuldade em pagar suas dívidas, já que suas receitas não estão sendo suficientes.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>E -) </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Imaginando que essa empresa foi constituída para comercializar mercadorias, quais ativos destinam-se a venda?</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:endParaRPr lang="pt-BR" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>R: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>O ativo que se destinaria a venda seria as mercadorias em estoque.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>F -) </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> Supondo que essa empresa está buscando obter um novo financiamento bancário, onde o banco empresta dinheiro apenas para as empresas cujo Patrimônio Líquido represente no mínimo 60% dos ativos. Nesse caso, a empresa ALFA vai conseguir obter o financiamento? Justifique.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>R:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> Considerando a situação dada, a empresa ALFA conseguiria obter o financiamento do banco tendo em vista que o Patrimônio Líquido ultrapassa os 60% de participação nos ativos totais.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2064,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16EA92BE-A10E-472B-B308-BE32DC980593}">
   <dimension ref="B1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2086,559 +1608,556 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="4"/>
-      <c r="K2" s="30" t="s">
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="75"/>
+      <c r="K2" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="32"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="78"/>
     </row>
     <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="72" t="s">
+      <c r="K3" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="73"/>
-      <c r="M3" s="28" t="s">
+      <c r="L3" s="54"/>
+      <c r="M3" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="29"/>
+      <c r="N3" s="25"/>
     </row>
     <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="5">
         <v>1000</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="39" t="s">
+      <c r="L4" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="50" t="s">
+      <c r="M4" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="N4" s="39" t="s">
+      <c r="N4" s="32" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="7">
         <v>200</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="K5" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="48">
+      <c r="L5" s="41">
         <v>500</v>
       </c>
-      <c r="M5" s="45" t="s">
+      <c r="M5" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="N5" s="48">
+      <c r="N5" s="41">
         <v>200</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="7">
         <v>500</v>
       </c>
-      <c r="K6" s="34" t="s">
+      <c r="K6" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="41">
+      <c r="L6" s="34">
         <v>100</v>
       </c>
-      <c r="M6" s="45" t="s">
+      <c r="M6" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="N6" s="71">
+      <c r="N6" s="52">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="7">
         <v>100</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="34" t="s">
+      <c r="K7" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="L7" s="40">
+      <c r="L7" s="33">
         <v>600</v>
       </c>
-      <c r="M7" s="45" t="s">
+      <c r="M7" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="N7" s="40">
+      <c r="N7" s="33">
         <v>400</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="7">
         <v>600</v>
       </c>
-      <c r="K8" s="33" t="s">
+      <c r="K8" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="41">
+      <c r="L8" s="34">
         <v>300</v>
       </c>
-      <c r="M8" s="45" t="s">
+      <c r="M8" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="42">
+      <c r="N8" s="35">
         <f>N5 - N6 + N7</f>
         <v>500</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="7">
         <v>300</v>
       </c>
-      <c r="K9" s="33" t="s">
+      <c r="K9" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="L9" s="41">
+      <c r="L9" s="34">
         <v>50</v>
       </c>
       <c r="M9" s="67"/>
-      <c r="N9" s="58"/>
+      <c r="N9" s="63"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="7">
         <v>50</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="33" t="s">
+      <c r="K10" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="L10" s="41">
+      <c r="L10" s="34">
         <v>300</v>
       </c>
-      <c r="M10" s="57"/>
-      <c r="N10" s="59"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="70"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="7">
         <v>300</v>
       </c>
-      <c r="K11" s="33" t="s">
+      <c r="K11" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="L11" s="42">
+      <c r="L11" s="35">
         <f>L5 - L6 + L7 - L8 -L9 -L10</f>
         <v>350</v>
       </c>
-      <c r="M11" s="57"/>
-      <c r="N11" s="59"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="70"/>
     </row>
     <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="10">
         <v>400</v>
       </c>
-      <c r="K12" s="35"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="59"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="70"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K13" s="50" t="s">
+      <c r="K13" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="L13" s="56"/>
-      <c r="M13" s="38" t="s">
+      <c r="L13" s="66"/>
+      <c r="M13" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="N13" s="64"/>
-    </row>
-    <row r="14" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K14" s="66" t="s">
+      <c r="N13" s="71"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K14" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="L14" s="49">
+      <c r="L14" s="42">
         <v>200</v>
       </c>
-      <c r="M14" s="45" t="s">
+      <c r="M14" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="N14" s="40">
+      <c r="N14" s="33">
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="79" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="81"/>
-      <c r="K15" s="36" t="s">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="K15" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="L15" s="43">
+      <c r="L15" s="36">
         <v>300</v>
       </c>
-      <c r="M15" s="46" t="s">
+      <c r="M15" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="N15" s="47">
+      <c r="N15" s="40">
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K16" s="36" t="s">
+      <c r="K16" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="L16" s="43">
+      <c r="L16" s="36">
         <v>400</v>
       </c>
-      <c r="M16" s="46" t="s">
+      <c r="M16" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="N16" s="44">
+      <c r="N16" s="37">
         <f>N14 - N15</f>
         <v>450</v>
       </c>
     </row>
     <row r="17" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="K17" s="36" t="s">
+      <c r="K17" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="L17" s="44">
+      <c r="L17" s="37">
         <f>SUM(L14:L16)</f>
         <v>900</v>
       </c>
-      <c r="M17" s="58"/>
-      <c r="N17" s="62"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="60"/>
     </row>
     <row r="18" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
         <v>58</v>
       </c>
-      <c r="K18" s="37"/>
-      <c r="L18" s="62"/>
-      <c r="M18" s="60"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="64"/>
       <c r="N18" s="61"/>
     </row>
     <row r="19" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="K19" s="26" t="s">
+      <c r="K19" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="L19" s="63"/>
-      <c r="M19" s="27" t="s">
+      <c r="L19" s="62"/>
+      <c r="M19" s="23" t="s">
         <v>50</v>
       </c>
       <c r="N19" s="61"/>
     </row>
     <row r="20" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="K20" s="36" t="s">
+      <c r="K20" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="L20" s="75">
+      <c r="L20" s="56">
         <v>1000</v>
       </c>
-      <c r="M20" s="69" t="s">
+      <c r="M20" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="N20" s="63"/>
+      <c r="N20" s="62"/>
     </row>
     <row r="21" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K21" s="37"/>
-      <c r="L21" s="62"/>
-      <c r="M21" s="52" t="s">
+      <c r="K21" s="30"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="N21" s="49">
+      <c r="N21" s="42">
         <v>1000</v>
       </c>
     </row>
     <row r="22" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="K22" s="26" t="s">
+      <c r="K22" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="L22" s="63"/>
-      <c r="M22" s="52" t="s">
+      <c r="L22" s="62"/>
+      <c r="M22" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="N22" s="43">
+      <c r="N22" s="36">
         <v>600</v>
       </c>
     </row>
     <row r="23" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="K23" s="36" t="s">
+      <c r="K23" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="L23" s="74">
+      <c r="L23" s="55">
         <v>300</v>
       </c>
-      <c r="M23" s="52" t="s">
+      <c r="M23" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="N23" s="44">
+      <c r="N23" s="37">
         <f>SUM(N21:N22)</f>
         <v>1600</v>
       </c>
     </row>
     <row r="24" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K24" s="53"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="76"/>
-      <c r="N24" s="65"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="48"/>
     </row>
     <row r="25" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K25" s="51" t="s">
+      <c r="K25" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="L25" s="77">
+      <c r="L25" s="58">
         <f>SUM(L11,L17,L20,L23)</f>
         <v>2550</v>
       </c>
-      <c r="M25" s="70" t="s">
+      <c r="M25" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="N25" s="78">
+      <c r="N25" s="59">
         <f>SUM(N16,N23,N8)</f>
         <v>2550</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="K2:N2"/>
     <mergeCell ref="N17:N20"/>
     <mergeCell ref="M17:M18"/>
-    <mergeCell ref="B15:I15"/>
     <mergeCell ref="L12:L13"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="M9:M12"/>
     <mergeCell ref="N9:N13"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="K2:N2"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F6">
     <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="↑">
@@ -2692,6 +2211,5 @@
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>